<commit_message>
update gzip figure and start analysis
</commit_message>
<xml_diff>
--- a/documentation/other-performance/gzip.xlsx
+++ b/documentation/other-performance/gzip.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/gzip/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/other-performance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A255402-1632-CA47-A67B-C33E6DEBD515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E0155A-304C-EE41-8246-A4B1DB112677}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-920" windowWidth="19200" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
+    <workbookView xWindow="52800" yWindow="-920" windowWidth="19200" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
   <sheets>
     <sheet name="gzip" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>QEMU</t>
   </si>
@@ -108,6 +108,47 @@
   </si>
   <si>
     <t>Post-pattern matching</t>
+  </si>
+  <si>
+    <r>
+      <t>v1.3.1-0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (523411b3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>v1.3.1-0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (523411b3)</t>
+    </r>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
@@ -199,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -234,17 +275,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -364,6 +394,71 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -379,95 +474,90 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -476,24 +566,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2E7EA3-8BF5-F743-9E89-1A0A4F76CDF3}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:G17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,64 +916,76 @@
     <col min="3" max="3" width="12.1640625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="7" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.4">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.4">
+      <c r="A1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-    </row>
-    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+    </row>
+    <row r="2" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-    </row>
-    <row r="3" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+    </row>
+    <row r="3" spans="1:10" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="30" t="s">
+      <c r="D4" s="37"/>
+      <c r="E4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="32"/>
-    </row>
-    <row r="5" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="F4" s="26"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="26"/>
+      <c r="J4" s="27"/>
+    </row>
+    <row r="5" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="33" t="s">
+      <c r="D5" s="39"/>
+      <c r="E5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="34"/>
-      <c r="G5" s="35"/>
-    </row>
-    <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="F5" s="29"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="29"/>
+      <c r="J5" s="30"/>
+    </row>
+    <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -887,378 +994,349 @@
       <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
+      <c r="H6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="44">
         <v>1</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="19">
         <v>44.405999999999999</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="20">
         <v>121.622</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="21">
         <f>$C7/$B7</f>
         <v>2.7388641174616044</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="22">
         <v>136.952</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="23">
         <f>$E7/$B7</f>
         <v>3.0840877358915462</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="24">
         <f>$E7/$C7</f>
         <v>1.1260462745227016</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
+      <c r="H7" s="22">
+        <v>84.403999999999996</v>
+      </c>
+      <c r="I7" s="23">
+        <f>$H7/$B7</f>
+        <v>1.9007341350267981</v>
+      </c>
+      <c r="J7" s="24">
+        <f>$H7/$C7</f>
+        <v>0.69398628537600104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="45">
         <v>2</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="19">
         <v>43.994999999999997</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="20">
         <v>125.071</v>
       </c>
-      <c r="D8" s="26">
-        <f t="shared" ref="D8:D16" si="0">$C8/$B8</f>
+      <c r="D8" s="21">
+        <f t="shared" ref="D8:D11" si="0">$C8/$B8</f>
         <v>2.8428457779293104</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="22">
         <v>136.74700000000001</v>
       </c>
-      <c r="F8" s="28">
-        <f t="shared" ref="F8:F16" si="1">$E8/$B8</f>
+      <c r="F8" s="23">
+        <f t="shared" ref="F8:F11" si="1">$E8/$B8</f>
         <v>3.108239572678714</v>
       </c>
-      <c r="G8" s="29">
-        <f t="shared" ref="G8:G16" si="2">$E8/$C8</f>
+      <c r="G8" s="24">
+        <f t="shared" ref="G8:G11" si="2">$E8/$C8</f>
         <v>1.0933549743745554</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="9">
+      <c r="H8" s="22">
+        <v>84.503</v>
+      </c>
+      <c r="I8" s="23">
+        <f t="shared" ref="I8:I11" si="3">$H8/$B8</f>
+        <v>1.9207409932946926</v>
+      </c>
+      <c r="J8" s="24">
+        <f t="shared" ref="J8:J11" si="4">$H8/$C8</f>
+        <v>0.67564023634575565</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="45">
         <v>3</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="19">
         <v>44.100999999999999</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="20">
         <v>121.21899999999999</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="21">
         <f t="shared" si="0"/>
         <v>2.7486678306614363</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="22">
         <v>136.494</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="23">
         <f t="shared" si="1"/>
         <v>3.0950318586880115</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="24">
         <f t="shared" si="2"/>
         <v>1.1260115988417658</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
+      <c r="H9" s="22">
+        <v>84.384</v>
+      </c>
+      <c r="I9" s="23">
+        <f t="shared" si="3"/>
+        <v>1.9134259994104443</v>
+      </c>
+      <c r="J9" s="24">
+        <f t="shared" si="4"/>
+        <v>0.69612849470792537</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="45">
         <v>4</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="19">
         <v>44.015000000000001</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="20">
         <v>121.426</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="21">
         <f t="shared" si="0"/>
         <v>2.7587413381801658</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="22">
         <v>136.69499999999999</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="23">
         <f t="shared" si="1"/>
         <v>3.1056458025673064</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="24">
         <f t="shared" si="2"/>
         <v>1.1257473687678092</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
+      <c r="H10" s="22">
+        <v>84.269000000000005</v>
+      </c>
+      <c r="I10" s="23">
+        <f t="shared" si="3"/>
+        <v>1.9145518573213678</v>
+      </c>
+      <c r="J10" s="24">
+        <f t="shared" si="4"/>
+        <v>0.69399469635827582</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="46">
         <v>5</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="19">
         <v>44.243000000000002</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="20">
         <v>121.529</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="21">
         <f t="shared" si="0"/>
         <v>2.7468526094523424</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="22">
         <v>136.518</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="23">
         <f t="shared" si="1"/>
         <v>3.0856406663200957</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="24">
         <f t="shared" si="2"/>
         <v>1.1233368167268718</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>6</v>
-      </c>
-      <c r="B12" s="24">
-        <v>44.545000000000002</v>
-      </c>
-      <c r="C12" s="25">
-        <v>122.09699999999999</v>
-      </c>
-      <c r="D12" s="26">
-        <f t="shared" si="0"/>
-        <v>2.7409810304186775</v>
-      </c>
-      <c r="E12" s="27">
-        <v>137.03100000000001</v>
-      </c>
-      <c r="F12" s="28">
-        <f t="shared" si="1"/>
-        <v>3.0762375126276797</v>
-      </c>
-      <c r="G12" s="29">
-        <f t="shared" si="2"/>
-        <v>1.1223125875328632</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>7</v>
-      </c>
-      <c r="B13" s="24">
-        <v>44.003999999999998</v>
-      </c>
-      <c r="C13" s="25">
-        <v>121.476</v>
-      </c>
-      <c r="D13" s="26">
-        <f t="shared" si="0"/>
-        <v>2.7605672211617125</v>
-      </c>
-      <c r="E13" s="27">
-        <v>136.99799999999999</v>
-      </c>
-      <c r="F13" s="28">
-        <f t="shared" si="1"/>
-        <v>3.1133078811017181</v>
-      </c>
-      <c r="G13" s="29">
-        <f t="shared" si="2"/>
-        <v>1.1277783265830286</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="9">
-        <v>8</v>
-      </c>
-      <c r="B14" s="24">
-        <v>43.771999999999998</v>
-      </c>
-      <c r="C14" s="25">
-        <v>121.414</v>
-      </c>
-      <c r="D14" s="26">
-        <f t="shared" si="0"/>
-        <v>2.7737823266014807</v>
-      </c>
-      <c r="E14" s="27">
-        <v>136.47200000000001</v>
-      </c>
-      <c r="F14" s="28">
-        <f t="shared" si="1"/>
-        <v>3.1177921959243355</v>
-      </c>
-      <c r="G14" s="29">
-        <f t="shared" si="2"/>
-        <v>1.1240219414565042</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
+      <c r="H11" s="22">
+        <v>84.393000000000001</v>
+      </c>
+      <c r="I11" s="23">
+        <f t="shared" si="3"/>
+        <v>1.9074881902221819</v>
+      </c>
+      <c r="J11" s="24">
+        <f t="shared" si="4"/>
+        <v>0.69442684462144844</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="24">
-        <v>44.319000000000003</v>
-      </c>
-      <c r="C15" s="25">
-        <v>121.015</v>
-      </c>
-      <c r="D15" s="26">
-        <f t="shared" si="0"/>
-        <v>2.7305444617432704</v>
-      </c>
-      <c r="E15" s="27">
-        <v>136.51400000000001</v>
-      </c>
-      <c r="F15" s="28">
-        <f t="shared" si="1"/>
-        <v>3.0802590311153231</v>
-      </c>
-      <c r="G15" s="29">
-        <f t="shared" si="2"/>
-        <v>1.1280750320208239</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>10</v>
-      </c>
-      <c r="B16" s="24">
-        <v>43.968000000000004</v>
-      </c>
-      <c r="C16" s="25">
-        <v>121.417</v>
-      </c>
-      <c r="D16" s="26">
-        <f t="shared" si="0"/>
-        <v>2.7614856259097524</v>
-      </c>
-      <c r="E16" s="27">
-        <v>137.292</v>
-      </c>
-      <c r="F16" s="28">
-        <f t="shared" si="1"/>
-        <v>3.1225436681222707</v>
-      </c>
-      <c r="G16" s="29">
-        <f t="shared" si="2"/>
-        <v>1.1307477536094617</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="20" t="s">
+      <c r="C12" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="D12" s="41"/>
+      <c r="E12" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="46"/>
-      <c r="E17" s="36" t="s">
+      <c r="F12" s="32"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="37"/>
-      <c r="G17" s="38"/>
-    </row>
-    <row r="18" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+      <c r="I12" s="32"/>
+      <c r="J12" s="33"/>
+    </row>
+    <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E13" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G13" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="4">
-        <f t="shared" ref="B19:G19" si="3">AVERAGE(B7:B16)</f>
-        <v>44.136800000000008</v>
-      </c>
-      <c r="C19" s="13">
-        <f t="shared" si="3"/>
-        <v>121.82859999999998</v>
-      </c>
-      <c r="D19" s="21">
-        <f t="shared" si="3"/>
-        <v>2.7603332339519753</v>
-      </c>
-      <c r="E19" s="17">
-        <f t="shared" si="3"/>
-        <v>136.77129999999997</v>
-      </c>
-      <c r="F19" s="21">
-        <f t="shared" si="3"/>
-        <v>3.0988785925036999</v>
-      </c>
-      <c r="G19" s="14">
-        <f t="shared" si="3"/>
-        <v>1.1227432674436386</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
+      <c r="H13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <f>AVERAGE(B7:B11)</f>
+        <v>44.152000000000001</v>
+      </c>
+      <c r="C14" s="8">
+        <f>AVERAGE(C7:C11)</f>
+        <v>122.17339999999999</v>
+      </c>
+      <c r="D14" s="16">
+        <f>AVERAGE(D7:D11)</f>
+        <v>2.7671943347369719</v>
+      </c>
+      <c r="E14" s="12">
+        <f>AVERAGE(E7:E11)</f>
+        <v>136.68119999999999</v>
+      </c>
+      <c r="F14" s="16">
+        <f>AVERAGE(F7:F11)</f>
+        <v>3.0957291272291347</v>
+      </c>
+      <c r="G14" s="9">
+        <f>AVERAGE(G7:G11)</f>
+        <v>1.1188994066467406</v>
+      </c>
+      <c r="H14" s="12">
+        <f>AVERAGE(H7:H11)</f>
+        <v>84.390599999999992</v>
+      </c>
+      <c r="I14" s="16">
+        <f>AVERAGE(I7:I11)</f>
+        <v>1.911388235055097</v>
+      </c>
+      <c r="J14" s="9">
+        <f>AVERAGE(J7:J11)</f>
+        <v>0.69083531148188126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="22" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C21" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="11">
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H12:J12"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E12:G12"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>